<commit_message>
LOG4J2-831 Fixed FAQ "which jars" diagrams: component name is JUL Adapter, not JUL Binding.
</commit_message>
<xml_diff>
--- a/src/site/resources/images/whichjar.xlsx
+++ b/src/site/resources/images/whichjar.xlsx
@@ -1215,11 +1215,11 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>JUL Bindi</a:t>
+            <a:t>JUL Adapter</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t> ng </a:t>
+            <a:t> </a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
         </a:p>
@@ -2187,7 +2187,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
LOG4J2-1156 2.4.1 web site corrections and updates
</commit_message>
<xml_diff>
--- a/src/site/resources/images/whichjar.xlsx
+++ b/src/site/resources/images/whichjar.xlsx
@@ -209,7 +209,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>(log4j-1.2-api-2.1.jar)</a:t>
+            <a:t>(log4j-1.2-api-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -273,7 +273,7 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
-            <a:t>2.1</a:t>
+            <a:t>2.x</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
@@ -284,7 +284,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
-            <a:t>(log4j-core-2.1.jar)</a:t>
+            <a:t>(log4j-core-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900"/>
         </a:p>
@@ -340,7 +340,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>Log4J 2.1</a:t>
+            <a:t>Log4J 2.x</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
@@ -351,7 +351,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t>(log4j-api-2.1.jar)</a:t>
+            <a:t>(log4j-api-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -419,7 +419,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>(log4j-slf4j-impl-2.1.jar)</a:t>
+            <a:t>(log4j-slf4j-impl-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -678,7 +678,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>(log4j-jcl-2.1.jar)</a:t>
+            <a:t>(log4j-jcl-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -843,7 +843,7 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>2.1</a:t>
+            <a:t>2.x</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
@@ -854,7 +854,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t>(log4j-api-2.1.jar)</a:t>
+            <a:t>(log4j-api-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -1227,7 +1227,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>(log4j-jul-2.1.jar)</a:t>
+            <a:t>(log4j-jul-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -1560,7 +1560,7 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
-            <a:t>2.1</a:t>
+            <a:t>2.x</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
@@ -1571,7 +1571,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t>(log4j-api-2.1.jar)</a:t>
+            <a:t>(log4j-api-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -1741,7 +1741,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t>(log4j-to-slf4j-2.1.jar)</a:t>
+            <a:t>(log4j-to-slf4j-2.x.jar)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
         </a:p>
@@ -2187,7 +2187,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2206,7 +2206,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
[DOC] Add images to migration page
</commit_message>
<xml_diff>
--- a/src/site/resources/images/whichjar.xlsx
+++ b/src/site/resources/images/whichjar.xlsx
@@ -1,34 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remko\IdeaProjects\logging-log4j2\src\site\resources\images\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AB1AC4-F5A7-4FE5-A844-101003844114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="19395" windowHeight="7830"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="whichjar-2.x" sheetId="1" r:id="rId1"/>
+    <sheet name="log4j-api" sheetId="5" r:id="rId2"/>
+    <sheet name="log4j-1.2-api" sheetId="4" r:id="rId3"/>
+    <sheet name="whichjar-slf4j-2.x" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -62,7 +70,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -70,6 +78,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -91,7 +102,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="正方形/長方形 10"/>
+        <xdr:cNvPr id="11" name="正方形/長方形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -149,25 +166,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>28574</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>586739</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>129300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="正方形/長方形 11"/>
+        <xdr:cNvPr id="12" name="正方形/長方形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2085975" y="762000"/>
-          <a:ext cx="1200150" cy="396000"/>
+          <a:off x="1857374" y="807720"/>
+          <a:ext cx="1167765" cy="418860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -232,7 +255,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+        <xdr:cNvPr id="13" name="正方形/長方形 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -307,7 +336,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="正方形/長方形 13"/>
+        <xdr:cNvPr id="14" name="正方形/長方形 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -362,25 +397,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:colOff>220981</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
+      <xdr:colOff>510541</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="正方形/長方形 17"/>
+        <xdr:cNvPr id="18" name="正方形/長方形 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4371975" y="1495424"/>
-          <a:ext cx="857249" cy="561975"/>
+          <a:off x="3878581" y="1586864"/>
+          <a:ext cx="899160" cy="596265"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -411,7 +452,7 @@
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
-            <a:t> ng </a:t>
+            <a:t>ng </a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
         </a:p>
@@ -430,25 +471,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>40005</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:colOff>135255</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>129300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="正方形/長方形 23"/>
+        <xdr:cNvPr id="24" name="正方形/長方形 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3438525" y="762000"/>
-          <a:ext cx="781050" cy="396000"/>
+          <a:off x="3088005" y="807720"/>
+          <a:ext cx="704850" cy="418860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -526,25 +573,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:colOff>236221</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>495301</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>129300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="正方形/長方形 33"/>
+        <xdr:cNvPr id="34" name="正方形/長方形 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000022000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4371975" y="762000"/>
-          <a:ext cx="847725" cy="396000"/>
+          <a:off x="3893821" y="807720"/>
+          <a:ext cx="868680" cy="418860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -626,25 +679,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>525780</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
+      <xdr:colOff>135254</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>161550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="正方形/長方形 34"/>
+        <xdr:cNvPr id="35" name="正方形/長方形 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000023000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3238500" y="1485900"/>
-          <a:ext cx="981074" cy="561600"/>
+          <a:off x="2964180" y="1577340"/>
+          <a:ext cx="828674" cy="595890"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -695,19 +754,25 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>129300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="正方形/長方形 35"/>
+        <xdr:cNvPr id="36" name="正方形/長方形 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5372101" y="762000"/>
-          <a:ext cx="971549" cy="396000"/>
+          <a:off x="4838701" y="807720"/>
+          <a:ext cx="967739" cy="418860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -790,7 +855,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>99060</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
@@ -798,17 +863,23 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>561975</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>129300</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="正方形/長方形 37"/>
+        <xdr:cNvPr id="38" name="正方形/長方形 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000026000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="885825" y="762000"/>
-          <a:ext cx="1047750" cy="396000"/>
+          <a:off x="708660" y="807720"/>
+          <a:ext cx="1072515" cy="411480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -865,27 +936,33 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>129300</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:colOff>25718</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>152398</xdr:rowOff>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="40" name="カギ線コネクタ 39"/>
+        <xdr:cNvPr id="40" name="カギ線コネクタ 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="38" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="712351" y="1855349"/>
-          <a:ext cx="1394698" cy="0"/>
+        <a:xfrm rot="5400000">
+          <a:off x="489109" y="1972151"/>
+          <a:ext cx="1508760" cy="2858"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -914,27 +991,33 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:colOff>605791</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>129300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2857</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="52" name="直線矢印コネクタ 51"/>
+        <xdr:cNvPr id="52" name="直線矢印コネクタ 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000034000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="12" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2686050" y="1158000"/>
-          <a:ext cx="0" cy="1204200"/>
+        <a:xfrm flipH="1">
+          <a:off x="2434591" y="1226580"/>
+          <a:ext cx="6666" cy="1284210"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -963,27 +1046,33 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>60960</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>60961</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="56" name="直線矢印コネクタ 55"/>
+        <xdr:cNvPr id="56" name="直線矢印コネクタ 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000038000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="18" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4800600" y="2057399"/>
-          <a:ext cx="0" cy="304801"/>
+        <a:xfrm flipH="1">
+          <a:off x="4328160" y="2183129"/>
+          <a:ext cx="1" cy="339091"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1024,7 +1113,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="58" name="直線矢印コネクタ 57"/>
+        <xdr:cNvPr id="58" name="直線矢印コネクタ 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1063,28 +1158,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>60961</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>129300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>681038</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>60961</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="60" name="直線矢印コネクタ 59"/>
+        <xdr:cNvPr id="60" name="直線矢印コネクタ 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="34" idx="2"/>
+          <a:endCxn id="18" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4795838" y="1158000"/>
-          <a:ext cx="0" cy="337425"/>
+          <a:off x="4328161" y="1226580"/>
+          <a:ext cx="0" cy="360284"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1130,7 +1232,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="62" name="直線矢印コネクタ 61"/>
+        <xdr:cNvPr id="62" name="直線矢印コネクタ 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1169,26 +1277,32 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="正方形/長方形 20"/>
+        <xdr:cNvPr id="21" name="正方形/長方形 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5419725" y="1495424"/>
-          <a:ext cx="857249" cy="561975"/>
+          <a:off x="4878705" y="1586864"/>
+          <a:ext cx="874395" cy="596265"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1250,7 +1364,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="直線矢印コネクタ 26"/>
+        <xdr:cNvPr id="27" name="直線矢印コネクタ 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1285,25 +1405,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:colOff>401955</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
+      <xdr:colOff>401955</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="28" name="直線矢印コネクタ 27"/>
+        <xdr:cNvPr id="28" name="直線矢印コネクタ 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3800475" y="2057399"/>
-          <a:ext cx="0" cy="304801"/>
+          <a:off x="3449955" y="2183129"/>
+          <a:ext cx="0" cy="327661"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1343,19 +1469,25 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>320040</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="正方形/長方形 1"/>
+        <xdr:cNvPr id="2" name="正方形/長方形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA9819BB-3147-455F-B0D4-05627C17631F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="704849" y="466725"/>
-          <a:ext cx="1409701" cy="571500"/>
+          <a:off x="628649" y="489585"/>
+          <a:ext cx="1520191" cy="617220"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1407,25 +1539,698 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:colOff>36195</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A972FCC7-9E55-4523-8012-2B9B97DBEF44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="645795" y="1586864"/>
+          <a:ext cx="1449705" cy="510541"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+            <a:t>Log4J</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+            <a:t>2.x</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
+            <a:t> Implementation</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
+            <a:t>(log4j-core-2.x.jar)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>74295</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="正方形/長方形 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FED5F0FE-B39D-4B0C-9F19-F912EA6A0B47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="830580" y="792480"/>
+          <a:ext cx="1072515" cy="411480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
+            <a:t>Log4J</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
+            <a:t>2.x</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
+            <a:t> API</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
+            <a:t>(log4j-api-2.x.jar)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>147638</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>151448</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="カギ線コネクタ 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4937D8C7-6CE1-4C0D-A154-34B5438FB0D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="2"/>
+          <a:endCxn id="4" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1177291" y="1393507"/>
+          <a:ext cx="382904" cy="3810"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6CF59B1-058D-4E1E-A7DB-A6225D93CED9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628649" y="489585"/>
+          <a:ext cx="2579371" cy="617220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+            <a:t>Application</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>81914</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>30479</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>129300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76F347CE-C56B-437B-9644-017020D01761}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1910714" y="807720"/>
+          <a:ext cx="1167765" cy="418860"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
+            <a:t>Log4J</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
+            <a:t> 1.2 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
+            <a:t>API</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
+            <a:t>(log4j-1.2-api-2.x.jar)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>607695</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>116204</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>78105</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{270A0B04-95EB-465E-B0AA-ADF200BDC416}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="607695" y="1945004"/>
+          <a:ext cx="2539365" cy="510541"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+            <a:t>Log4J</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+            <a:t>2.x</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
+            <a:t> Implementation</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
+            <a:t>(log4j-core-2.x.jar)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>131445</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>87629</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>20954</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46EF553F-2D69-48FE-9313-B1CE9B2E6909}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1960245" y="1733549"/>
+          <a:ext cx="1072515" cy="481965"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1"/>
+            <a:t>Log4J 2.x</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
+            <a:t> API</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" i="1" baseline="0"/>
+            <a:t>(log4j-api-2.x.jar)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>56197</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>129300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>58103</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>87629</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="直線矢印コネクタ 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF8FED5E-9918-4DDE-9320-611692E2650F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="2"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2494597" y="1226580"/>
+          <a:ext cx="1906" cy="506969"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704849" y="466725"/>
+          <a:ext cx="1409701" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+            <a:t>Application</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>148590</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>15000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="正方形/長方形 7"/>
+        <xdr:cNvPr id="8" name="正方形/長方形 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="981075" y="2190750"/>
-          <a:ext cx="847725" cy="396000"/>
+          <a:off x="758190" y="2327910"/>
+          <a:ext cx="1032510" cy="430290"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1507,25 +2312,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
+      <xdr:colOff>115253</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
+      <xdr:colOff>608648</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>129300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="正方形/長方形 11"/>
+        <xdr:cNvPr id="12" name="正方形/長方形 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="885825" y="762000"/>
-          <a:ext cx="1047750" cy="396000"/>
+          <a:off x="724853" y="807720"/>
+          <a:ext cx="1102995" cy="418860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1582,19 +2393,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>44451</xdr:colOff>
+      <xdr:colOff>57151</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>135649</xdr:rowOff>
+      <xdr:rowOff>129300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>44451</xdr:colOff>
+      <xdr:colOff>57152</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>111124</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="13" name="カギ線コネクタ 12"/>
+        <xdr:cNvPr id="13" name="カギ線コネクタ 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="12" idx="2"/>
           <a:endCxn id="21" idx="0"/>
@@ -1602,8 +2419,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1256863" y="1323537"/>
-          <a:ext cx="318375" cy="0"/>
+          <a:off x="1105734" y="1397197"/>
+          <a:ext cx="341235" cy="1"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1634,19 +2451,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>33338</xdr:colOff>
+      <xdr:colOff>55245</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>15000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>33338</xdr:colOff>
+      <xdr:colOff>57151</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="直線矢印コネクタ 17"/>
+        <xdr:cNvPr id="18" name="直線矢印コネクタ 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="8" idx="2"/>
           <a:endCxn id="26" idx="0"/>
@@ -1654,8 +2477,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1404938" y="2586750"/>
-          <a:ext cx="0" cy="318375"/>
+          <a:off x="1274445" y="2758200"/>
+          <a:ext cx="1906" cy="329805"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1689,25 +2512,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>45720</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>157875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="正方形/長方形 20"/>
+        <xdr:cNvPr id="21" name="正方形/長方形 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="809625" y="1476375"/>
-          <a:ext cx="1200150" cy="396000"/>
+          <a:off x="655320" y="1567815"/>
+          <a:ext cx="1242060" cy="418860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1752,25 +2581,31 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:colOff>118111</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
+      <xdr:colOff>605790</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>43575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="正方形/長方形 25"/>
+        <xdr:cNvPr id="26" name="正方形/長方形 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="923925" y="2905125"/>
-          <a:ext cx="962025" cy="396000"/>
+          <a:off x="727711" y="3088005"/>
+          <a:ext cx="1097279" cy="430290"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1845,19 +2680,25 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>38101</xdr:colOff>
+      <xdr:colOff>55246</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>157874</xdr:rowOff>
+      <xdr:rowOff>157875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>38101</xdr:colOff>
+      <xdr:colOff>57151</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="カギ線コネクタ 26"/>
+        <xdr:cNvPr id="25" name="カギ線コネクタ 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3140FD44-A960-4B5B-8692-B08EEBDB292C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="21" idx="2"/>
           <a:endCxn id="8" idx="0"/>
@@ -1865,8 +2706,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1250513" y="2031562"/>
-          <a:ext cx="318375" cy="0"/>
+          <a:off x="1104781" y="2156340"/>
+          <a:ext cx="341235" cy="1905"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1898,7 +2739,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1940,7 +2781,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1973,9 +2814,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2008,6 +2866,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2183,14 +3058,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2202,14 +3077,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAAA7017-C7E9-4141-9F88-BCB6AEFACAC3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05553D8D-B041-4F6E-9B9B-4DF6D47C6E34}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2217,13 +3122,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>